<commit_message>
March 2023 updated numbers
</commit_message>
<xml_diff>
--- a/imaging_by_the_numbers_by_subject_2.xlsx
+++ b/imaging_by_the_numbers_by_subject_2.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ermcg\Box\abcd2_data_wrangling_Jan2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilymcgrew/git_repos/abcd2_data_wrangling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EEA9FB2-E0EB-4A9B-B986-F37CEAB00487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442BDF4B-4B3A-5C49-89E3-227840878F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29955" yWindow="1635" windowWidth="19920" windowHeight="14295" xr2:uid="{A4D822DD-2E57-4CE2-AF3D-D24377A280AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A4D822DD-2E57-4CE2-AF3D-D24377A280AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="20230112" sheetId="1" r:id="rId1"/>
+    <sheet name="20230313" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Subjects with scans by study</t>
   </si>
@@ -72,6 +76,24 @@
   </si>
   <si>
     <t xml:space="preserve">     ABC &amp; ABCD2 Amyloid negative</t>
+  </si>
+  <si>
+    <t>Total ABCD2 sessions: 19</t>
+  </si>
+  <si>
+    <t>3T sessions: 7</t>
+  </si>
+  <si>
+    <t>Amyloid PET sessions: 6</t>
+  </si>
+  <si>
+    <t>Tau PET sessions: 6</t>
+  </si>
+  <si>
+    <t>Number of subejcts: 16</t>
+  </si>
+  <si>
+    <t>Since January 1, 2023</t>
   </si>
 </sst>
 </file>
@@ -255,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,7 +301,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,18 +627,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFC1F02-31B7-4ACE-BE5A-2E7CBF4B7739}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -620,7 +653,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -634,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -648,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -662,7 +695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -676,7 +709,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -690,7 +723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -704,7 +737,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -720,9 +753,8 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -739,7 +771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -754,6 +786,210 @@
       <c r="D10" s="10">
         <f t="shared" si="2"/>
         <v>81</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="14"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H1:H19">
+    <sortCondition ref="H1:H19"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D745B5-22AE-1F48-9A29-34FC0A3C44F1}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="18">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19">
+        <v>25</v>
+      </c>
+      <c r="D2" s="20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>423</v>
+      </c>
+      <c r="C5" s="8">
+        <v>240</v>
+      </c>
+      <c r="D5" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>149</v>
+      </c>
+      <c r="C6" s="9">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>148</v>
+      </c>
+      <c r="C7" s="10">
+        <v>127</v>
+      </c>
+      <c r="D7" s="5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>SUM(B2,B5)</f>
+        <v>456</v>
+      </c>
+      <c r="C8" s="8">
+        <f t="shared" ref="C8:D10" si="0">SUM(C2,C5)</f>
+        <v>265</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <f>SUM(B3,B6)</f>
+        <v>149</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <f>SUM(B4,B7)</f>
+        <v>165</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>142</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>